<commit_message>
changes to xml lab 1
</commit_message>
<xml_diff>
--- a/Lab 1/Lab01_Review Form_Filled.xlsx
+++ b/Lab 1/Lab01_Review Form_Filled.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements Phase Defects" sheetId="7" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="38">
   <si>
     <t>Document  Title:</t>
   </si>
@@ -129,44 +129,6 @@
   </si>
   <si>
     <t>FR2 – Behavior if category not found</t>
-  </si>
-  <si>
-    <t>Actors – Should The Salesperson alter the 
-Product quantity? as it is a great responsibility 
-and probably the manager/owner 
-Should handle this</t>
-  </si>
-  <si>
-    <t>Use Case – No Use Case for Invalid members\</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Attributes – Since both Name and Code are 
-uniquely identifiers, what should be the 
-Primary key? </t>
-  </si>
-  <si>
-    <t>System behavior – Opt 4 – Product Exists 
-(switch yes/no), because if product does not 
-Exist we cannot print it</t>
-  </si>
-  <si>
-    <t>Use case 2 &amp; 3 are duplicates – Use case 2 
-should be get products by category</t>
-  </si>
-  <si>
-    <t>Use case 4 – there should be 1 product, not a list</t>
-  </si>
-  <si>
-    <t>StoreRepository &amp; StoreController– 
-stockSituationProduct – 
-Parameter incorrect naming</t>
-  </si>
-  <si>
-    <t>Design should not be in Requirements file</t>
-  </si>
-  <si>
-    <t>GRASP – Implementation info should not be
-In the Requirements file</t>
   </si>
   <si>
     <t>Store Inventory</t>
@@ -653,8 +615,8 @@
   </sheetPr>
   <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView topLeftCell="A78" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="E17" sqref="C17:E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -683,7 +645,7 @@
         <v>0</v>
       </c>
       <c r="D4" s="17" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="E4" s="17"/>
     </row>
@@ -693,7 +655,7 @@
         <v>3</v>
       </c>
       <c r="D5" s="17" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="E5" s="17"/>
     </row>
@@ -748,140 +710,86 @@
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B11" s="3">
         <f t="shared" ref="B11:B24" si="0">B10+1</f>
         <v>3</v>
       </c>
-      <c r="C11" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="D11" s="12">
-        <v>3</v>
-      </c>
-      <c r="E11" s="13" t="s">
-        <v>36</v>
-      </c>
+      <c r="C11" s="12"/>
+      <c r="D11" s="12"/>
+      <c r="E11" s="13"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B12" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="C12" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="D12" s="12">
-        <v>4</v>
-      </c>
-      <c r="E12" s="12" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="C12" s="12"/>
+      <c r="D12" s="12"/>
+      <c r="E12" s="12"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B13" s="3">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="C13" t="s">
-        <v>15</v>
-      </c>
-      <c r="D13">
+      <c r="C13"/>
+      <c r="D13"/>
+      <c r="E13" s="14"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B14" s="3">
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="E13" s="14" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="B14" s="3">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="C14" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="D14" s="12">
+      <c r="C14" s="12"/>
+      <c r="D14" s="12"/>
+      <c r="E14" s="13"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B15" s="3">
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="E14" s="13" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B15" s="3">
-        <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="C15" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="D15" s="12">
-        <v>7</v>
-      </c>
-      <c r="E15" s="13" t="s">
-        <v>40</v>
-      </c>
+      <c r="C15" s="12"/>
+      <c r="D15" s="12"/>
+      <c r="E15" s="13"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B16" s="3">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="C16" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="D16" s="12">
-        <v>8</v>
-      </c>
-      <c r="E16" s="12" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="17" spans="2:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="C16" s="12"/>
+      <c r="D16" s="12"/>
+      <c r="E16" s="12"/>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B17" s="3">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="C17" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="D17" s="12">
-        <v>9</v>
-      </c>
-      <c r="E17" s="13" t="s">
-        <v>42</v>
-      </c>
+      <c r="C17" s="12"/>
+      <c r="D17" s="12"/>
+      <c r="E17" s="13"/>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B18" s="3">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="C18" s="12" t="s">
+      <c r="C18" s="12"/>
+      <c r="D18" s="12"/>
+      <c r="E18" s="12"/>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B19" s="3">
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="D18" s="12">
-        <v>8</v>
-      </c>
-      <c r="E18" s="12" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="19" spans="2:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B19" s="3">
-        <f t="shared" si="0"/>
-        <v>11</v>
-      </c>
-      <c r="C19" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="D19" s="12">
-        <v>11</v>
-      </c>
-      <c r="E19" s="13" t="s">
-        <v>44</v>
-      </c>
+      <c r="C19" s="12"/>
+      <c r="D19" s="12"/>
+      <c r="E19" s="13"/>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B20" s="3">
@@ -958,7 +866,7 @@
   </sheetPr>
   <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+    <sheetView topLeftCell="A8" workbookViewId="0">
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
@@ -988,7 +896,7 @@
         <v>0</v>
       </c>
       <c r="D4" s="17" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="E4" s="17"/>
     </row>
@@ -998,7 +906,7 @@
         <v>3</v>
       </c>
       <c r="D5" s="17" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="E5" s="17"/>
     </row>
@@ -1297,7 +1205,7 @@
         <v>0</v>
       </c>
       <c r="D4" s="17" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="E4" s="17"/>
     </row>
@@ -1307,7 +1215,7 @@
         <v>3</v>
       </c>
       <c r="D5" s="17" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="E5" s="17"/>
     </row>

</xml_diff>